<commit_message>
updated poets_cities to recover notes
</commit_message>
<xml_diff>
--- a/production/data/poets_cities.xlsx
+++ b/production/data/poets_cities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
+    <workbookView xWindow="13920" yWindow="-20" windowWidth="13920" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="poets" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="267">
   <si>
     <t>Melanippides</t>
   </si>
@@ -880,15 +880,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -960,7 +954,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="56">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -989,9 +983,6 @@
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1019,9 +1010,6 @@
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1292,7 +1280,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1302,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E254" sqref="E254"/>
+    <sheetView tabSelected="1" topLeftCell="A243" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C262" sqref="C262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1403,6 +1391,9 @@
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="G4" t="s">
+        <v>194</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="2"/>
     </row>
@@ -1423,6 +1414,9 @@
       <c r="F5">
         <v>3</v>
       </c>
+      <c r="G5" t="s">
+        <v>249</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="2"/>
     </row>
@@ -1443,6 +1437,9 @@
       <c r="F6">
         <v>1</v>
       </c>
+      <c r="G6" t="s">
+        <v>218</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
     </row>
@@ -1531,9 +1528,6 @@
       <c r="F10">
         <v>3</v>
       </c>
-      <c r="G10" t="s">
-        <v>131</v>
-      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
     </row>
@@ -1665,9 +1659,6 @@
       <c r="F16">
         <v>3</v>
       </c>
-      <c r="G16" t="s">
-        <v>132</v>
-      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
     </row>
@@ -1708,6 +1699,9 @@
       <c r="F18">
         <v>1</v>
       </c>
+      <c r="G18" t="s">
+        <v>212</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="2"/>
     </row>
@@ -1753,6 +1747,9 @@
       <c r="F20">
         <v>1</v>
       </c>
+      <c r="G20" t="s">
+        <v>212</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="2"/>
     </row>
@@ -1792,6 +1789,9 @@
       <c r="F22">
         <v>1</v>
       </c>
+      <c r="G22" t="s">
+        <v>131</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="2"/>
     </row>
@@ -1858,6 +1858,9 @@
       <c r="F25">
         <v>3</v>
       </c>
+      <c r="G25" t="s">
+        <v>212</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="2"/>
     </row>
@@ -1878,6 +1881,9 @@
       <c r="F26">
         <v>3</v>
       </c>
+      <c r="G26" t="s">
+        <v>212</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="2"/>
     </row>
@@ -1918,6 +1924,9 @@
       <c r="F28">
         <v>3</v>
       </c>
+      <c r="G28" t="s">
+        <v>212</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="2"/>
     </row>
@@ -2003,6 +2012,9 @@
       <c r="F32">
         <v>3</v>
       </c>
+      <c r="G32" t="s">
+        <v>250</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="2"/>
     </row>
@@ -2023,6 +2035,9 @@
       <c r="F33">
         <v>3</v>
       </c>
+      <c r="G33" t="s">
+        <v>212</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="2"/>
     </row>
@@ -2170,6 +2185,9 @@
       <c r="F40">
         <v>1</v>
       </c>
+      <c r="G40" t="s">
+        <v>132</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="2"/>
     </row>
@@ -2564,9 +2582,6 @@
       <c r="F59">
         <v>1</v>
       </c>
-      <c r="G59" t="s">
-        <v>130</v>
-      </c>
       <c r="I59" s="2"/>
     </row>
     <row r="60" spans="1:9">
@@ -2655,6 +2670,9 @@
       <c r="F63">
         <v>1</v>
       </c>
+      <c r="G63" t="s">
+        <v>212</v>
+      </c>
       <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9">
@@ -2854,7 +2872,6 @@
       <c r="F73">
         <v>1</v>
       </c>
-      <c r="G73" s="1"/>
       <c r="H73" s="3"/>
       <c r="I73" s="2"/>
     </row>
@@ -2874,7 +2891,6 @@
       <c r="F74">
         <v>3</v>
       </c>
-      <c r="G74" s="1"/>
       <c r="I74" s="2"/>
     </row>
     <row r="75" spans="1:9">
@@ -2896,7 +2912,6 @@
       <c r="F75">
         <v>1</v>
       </c>
-      <c r="G75" s="1"/>
       <c r="H75" s="3"/>
       <c r="I75" s="2"/>
     </row>
@@ -2958,9 +2973,6 @@
       <c r="F78">
         <v>1</v>
       </c>
-      <c r="G78" t="s">
-        <v>134</v>
-      </c>
       <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9">
@@ -3002,6 +3014,9 @@
       <c r="F80">
         <v>1</v>
       </c>
+      <c r="G80" t="s">
+        <v>212</v>
+      </c>
       <c r="I80" s="2"/>
     </row>
     <row r="81" spans="1:9">
@@ -3082,9 +3097,6 @@
       <c r="F84">
         <v>3</v>
       </c>
-      <c r="G84" t="s">
-        <v>133</v>
-      </c>
       <c r="H84" s="3"/>
       <c r="I84" s="2"/>
     </row>
@@ -3242,6 +3254,9 @@
       <c r="F92">
         <v>3</v>
       </c>
+      <c r="G92" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
@@ -3281,37 +3296,42 @@
       <c r="F94">
         <v>3</v>
       </c>
+      <c r="G94" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" t="s">
-        <v>155</v>
-      </c>
-      <c r="B95" s="2">
-        <f>VLOOKUP(A95,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>114</v>
-      </c>
-      <c r="C95" t="s">
-        <v>2</v>
+      <c r="A95" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B95">
+        <v>67</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D95">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="F95">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B96">
-        <v>67</v>
-      </c>
-      <c r="C96" s="3" t="s">
+      <c r="A96" t="s">
+        <v>59</v>
+      </c>
+      <c r="B96" s="2">
+        <v>42</v>
+      </c>
+      <c r="C96" t="s">
         <v>3</v>
       </c>
       <c r="D96">
         <v>2</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -3325,16 +3345,16 @@
         <v>42</v>
       </c>
       <c r="C97" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="D97">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F97">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3345,10 +3365,10 @@
         <v>42</v>
       </c>
       <c r="C98" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D98">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>87</v>
@@ -3358,74 +3378,75 @@
       </c>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" t="s">
-        <v>59</v>
-      </c>
-      <c r="B99" s="2">
-        <v>42</v>
-      </c>
-      <c r="C99" t="s">
-        <v>74</v>
+      <c r="A99" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99">
+        <v>68</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D99">
-        <v>10</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="F99">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B100">
-        <v>68</v>
-      </c>
-      <c r="C100" s="3" t="s">
+      <c r="A100" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100" s="2">
+        <v>12</v>
+      </c>
+      <c r="C100" t="s">
         <v>3</v>
       </c>
       <c r="D100">
         <v>2</v>
       </c>
+      <c r="E100" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="F100">
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" t="s">
-        <v>20</v>
-      </c>
-      <c r="B101" s="2">
-        <v>12</v>
-      </c>
-      <c r="C101" t="s">
-        <v>3</v>
+      <c r="A101" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101">
+        <v>69</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="D101">
-        <v>2</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F101">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B102">
-        <v>69</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>110</v>
+      <c r="A102" t="s">
+        <v>156</v>
+      </c>
+      <c r="B102" s="2">
+        <f>VLOOKUP(A102,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>115</v>
+      </c>
+      <c r="C102" t="s">
+        <v>3</v>
       </c>
       <c r="D102">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -3440,65 +3461,65 @@
         <v>115</v>
       </c>
       <c r="C103" t="s">
-        <v>3</v>
+        <v>255</v>
       </c>
       <c r="D103">
-        <v>2</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F103">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" t="s">
-        <v>156</v>
-      </c>
-      <c r="B104" s="2">
-        <f>VLOOKUP(A104,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>115</v>
-      </c>
-      <c r="C104" t="s">
-        <v>255</v>
+      <c r="A104" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B104">
+        <v>70</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D104">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="F104">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B105">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D105">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F105">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B106">
-        <v>71</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>63</v>
+      <c r="A106" t="s">
+        <v>157</v>
+      </c>
+      <c r="B106" s="2">
+        <f>VLOOKUP(A106,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>116</v>
+      </c>
+      <c r="C106" t="s">
+        <v>36</v>
       </c>
       <c r="D106">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3513,34 +3534,34 @@
         <v>116</v>
       </c>
       <c r="C107" t="s">
-        <v>36</v>
+        <v>235</v>
       </c>
       <c r="D107">
-        <v>11</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F107">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B108" s="2">
         <f>VLOOKUP(A108,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C108" t="s">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="D108">
-        <v>75</v>
+        <v>15</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F108">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3552,16 +3573,16 @@
         <v>117</v>
       </c>
       <c r="C109" t="s">
-        <v>42</v>
+        <v>220</v>
       </c>
       <c r="D109">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F109">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3573,76 +3594,72 @@
         <v>117</v>
       </c>
       <c r="C110" t="s">
-        <v>220</v>
+        <v>114</v>
       </c>
       <c r="D110">
-        <v>49</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="F110">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:6">
-      <c r="A111" t="s">
-        <v>158</v>
-      </c>
-      <c r="B111" s="2">
-        <f>VLOOKUP(A111,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>117</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="A111" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B111">
+        <v>72</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D111">
         <v>41</v>
       </c>
       <c r="F111">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:6">
-      <c r="A112" s="3" t="s">
-        <v>203</v>
+      <c r="A112" t="s">
+        <v>202</v>
       </c>
       <c r="B112">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="D112">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="F112">
         <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:7">
-      <c r="A113" s="3" t="s">
+      <c r="A113" t="s">
         <v>202</v>
       </c>
       <c r="B113">
         <v>55</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D113">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F113">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="3" t="s">
-        <v>202</v>
+        <v>115</v>
       </c>
       <c r="B114">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>3</v>
@@ -3651,44 +3668,47 @@
         <v>2</v>
       </c>
       <c r="F114">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:7">
-      <c r="A115" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B115">
-        <v>73</v>
-      </c>
-      <c r="C115" s="3" t="s">
+      <c r="A115" t="s">
+        <v>21</v>
+      </c>
+      <c r="B115" s="2">
+        <v>13</v>
+      </c>
+      <c r="C115" t="s">
         <v>3</v>
       </c>
       <c r="D115">
         <v>2</v>
       </c>
+      <c r="E115" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F115">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B116" s="2">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C116" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F116">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3699,16 +3719,16 @@
         <v>51</v>
       </c>
       <c r="C117" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D117">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F117">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3719,10 +3739,10 @@
         <v>51</v>
       </c>
       <c r="C118" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="D118">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>87</v>
@@ -3733,10 +3753,10 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="B119" s="2">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="C119" t="s">
         <v>3</v>
@@ -3745,67 +3765,64 @@
         <v>2</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F119">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:7">
-      <c r="A120" t="s">
-        <v>22</v>
-      </c>
-      <c r="B120" s="2">
-        <v>14</v>
-      </c>
-      <c r="C120" t="s">
-        <v>3</v>
+      <c r="A120" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B120">
+        <v>75</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D120">
-        <v>2</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="F120">
         <v>1</v>
       </c>
       <c r="G120" t="s">
-        <v>194</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B121">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D121">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F121">
         <v>1</v>
       </c>
-      <c r="G121" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="122" spans="1:7">
-      <c r="A122" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B122">
-        <v>76</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>42</v>
+      <c r="A122" t="s">
+        <v>65</v>
+      </c>
+      <c r="B122" s="2">
+        <v>46</v>
+      </c>
+      <c r="C122" t="s">
+        <v>3</v>
       </c>
       <c r="D122">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -3813,16 +3830,16 @@
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="B123" s="2">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C123" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D123">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>85</v>
@@ -3839,39 +3856,36 @@
         <v>20</v>
       </c>
       <c r="C124" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D124">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F124">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="B125" s="2">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C125" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="D125">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F125">
-        <v>3</v>
-      </c>
-      <c r="G125" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3882,27 +3896,25 @@
         <v>47</v>
       </c>
       <c r="C126" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="D126">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F126">
-        <v>1</v>
-      </c>
-      <c r="G126" t="s">
-        <v>212</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="B127" s="2">
-        <v>47</v>
+        <f>VLOOKUP(A127,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>119</v>
       </c>
       <c r="C127" t="s">
         <v>3</v>
@@ -3911,31 +3923,34 @@
         <v>2</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F127">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B128" s="2">
         <f>VLOOKUP(A128,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C128" t="s">
-        <v>3</v>
+        <v>222</v>
       </c>
       <c r="D128">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F128">
         <v>1</v>
+      </c>
+      <c r="G128" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3947,48 +3962,48 @@
         <v>120</v>
       </c>
       <c r="C129" t="s">
-        <v>222</v>
+        <v>3</v>
       </c>
       <c r="D129">
-        <v>50</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="F129">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" t="s">
-        <v>160</v>
+        <v>43</v>
       </c>
       <c r="B130" s="2">
-        <f>VLOOKUP(A130,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="C130" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D130">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F130">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="B131" s="2">
-        <v>28</v>
+        <f>VLOOKUP(A131,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>121</v>
       </c>
       <c r="C131" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D131">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>85</v>
@@ -4006,16 +4021,13 @@
         <v>121</v>
       </c>
       <c r="C132" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="D132">
-        <v>31</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="F132">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -4027,10 +4039,10 @@
         <v>121</v>
       </c>
       <c r="C133" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D133">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F133">
         <v>3</v>
@@ -4038,20 +4050,22 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>161</v>
+        <v>6</v>
       </c>
       <c r="B134" s="2">
-        <f>VLOOKUP(A134,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>121</v>
+        <v>3</v>
       </c>
       <c r="C134" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D134">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F134">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4062,16 +4076,16 @@
         <v>3</v>
       </c>
       <c r="C135" t="s">
+        <v>73</v>
+      </c>
+      <c r="D135">
         <v>7</v>
       </c>
-      <c r="D135">
-        <v>6</v>
-      </c>
       <c r="E135" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F135">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4082,10 +4096,10 @@
         <v>3</v>
       </c>
       <c r="C136" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="D136">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>87</v>
@@ -4093,28 +4107,22 @@
       <c r="F136">
         <v>3</v>
       </c>
-      <c r="G136" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="137" spans="1:7">
-      <c r="A137" t="s">
-        <v>6</v>
-      </c>
-      <c r="B137" s="2">
-        <v>3</v>
-      </c>
-      <c r="C137" t="s">
-        <v>3</v>
+      <c r="A137" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B137">
+        <v>52</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="D137">
-        <v>2</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="F137">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -4125,13 +4133,13 @@
         <v>52</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="D138">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F138">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -4142,34 +4150,36 @@
         <v>52</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D139">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F139">
         <v>3</v>
       </c>
-      <c r="G139" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="140" spans="1:7">
-      <c r="A140" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B140">
-        <v>52</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>127</v>
+      <c r="A140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
+        <v>1</v>
       </c>
       <c r="D140">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F140">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G140" s="1"/>
     </row>
     <row r="141" spans="1:7">
       <c r="A141" t="s">
@@ -4180,17 +4190,18 @@
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D141">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F141">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G141" s="1"/>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" t="s">
@@ -4201,88 +4212,92 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D142">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F142">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G142" s="1"/>
     </row>
     <row r="143" spans="1:7">
-      <c r="A143" t="s">
-        <v>0</v>
-      </c>
-      <c r="B143" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="C143" t="s">
-        <v>3</v>
-      </c>
-      <c r="D143">
-        <v>2</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>87</v>
+      <c r="A143" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B143">
+        <v>91</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D143" s="3">
+        <v>2</v>
       </c>
       <c r="F143">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:7">
-      <c r="A144" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B144">
-        <v>91</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D144" s="3">
-        <v>2</v>
+      <c r="A144" t="s">
+        <v>68</v>
+      </c>
+      <c r="B144" s="2">
+        <v>48</v>
+      </c>
+      <c r="C144" t="s">
+        <v>3</v>
+      </c>
+      <c r="D144">
+        <v>2</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F144">
         <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:7">
-      <c r="A145" t="s">
-        <v>68</v>
-      </c>
-      <c r="B145" s="2">
-        <v>48</v>
-      </c>
-      <c r="C145" t="s">
+      <c r="A145" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B145">
+        <v>53</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D145">
         <v>2</v>
       </c>
-      <c r="E145" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F145">
         <v>1</v>
       </c>
+      <c r="G145" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="146" spans="1:7">
-      <c r="A146" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B146">
-        <v>53</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>3</v>
+      <c r="A146" t="s">
+        <v>162</v>
+      </c>
+      <c r="B146" s="2">
+        <f>VLOOKUP(A146,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>122</v>
+      </c>
+      <c r="C146" t="s">
+        <v>78</v>
       </c>
       <c r="D146">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F146">
         <v>1</v>
@@ -4297,10 +4312,10 @@
         <v>122</v>
       </c>
       <c r="C147" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D147">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>85</v>
@@ -4318,54 +4333,53 @@
         <v>122</v>
       </c>
       <c r="C148" t="s">
-        <v>92</v>
+        <v>223</v>
       </c>
       <c r="D148">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F148">
         <v>1</v>
+      </c>
+      <c r="G148" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="B149" s="2">
-        <f>VLOOKUP(A149,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="C149" t="s">
-        <v>223</v>
+        <v>3</v>
       </c>
       <c r="D149">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F149">
-        <v>1</v>
-      </c>
-      <c r="G149" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:7">
-      <c r="A150" t="s">
+      <c r="A150" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B150" s="2">
         <v>49</v>
       </c>
-      <c r="C150" t="s">
-        <v>3</v>
+      <c r="C150" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D150">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>87</v>
@@ -4375,52 +4389,52 @@
       </c>
     </row>
     <row r="151" spans="1:7">
-      <c r="A151" s="4" t="s">
-        <v>69</v>
+      <c r="A151" t="s">
+        <v>163</v>
       </c>
       <c r="B151" s="2">
-        <v>49</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>56</v>
+        <f>VLOOKUP(A151,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>123</v>
+      </c>
+      <c r="C151" t="s">
+        <v>191</v>
       </c>
       <c r="D151">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F151">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:7">
       <c r="A152" t="s">
-        <v>163</v>
+        <v>23</v>
       </c>
       <c r="B152" s="2">
-        <f>VLOOKUP(A152,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="C152" t="s">
-        <v>191</v>
+        <v>3</v>
       </c>
       <c r="D152">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F152">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:7">
       <c r="A153" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B153" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C153" t="s">
         <v>3</v>
@@ -4434,16 +4448,13 @@
       <c r="F153">
         <v>3</v>
       </c>
-      <c r="G153" t="s">
-        <v>215</v>
-      </c>
     </row>
     <row r="154" spans="1:7">
       <c r="A154" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B154" s="2">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C154" t="s">
         <v>3</v>
@@ -4459,90 +4470,94 @@
       </c>
     </row>
     <row r="155" spans="1:7">
-      <c r="A155" t="s">
-        <v>44</v>
-      </c>
-      <c r="B155" s="2">
-        <v>29</v>
-      </c>
-      <c r="C155" t="s">
-        <v>3</v>
-      </c>
-      <c r="D155">
-        <v>2</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="A155" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B155">
+        <v>78</v>
+      </c>
+      <c r="C155" s="3"/>
       <c r="F155">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G155" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="156" spans="1:7">
-      <c r="A156" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B156">
-        <v>78</v>
-      </c>
-      <c r="C156" s="3"/>
+      <c r="A156" t="s">
+        <v>164</v>
+      </c>
+      <c r="B156" s="2">
+        <f>VLOOKUP(A156,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>124</v>
+      </c>
+      <c r="C156" t="s">
+        <v>224</v>
+      </c>
+      <c r="D156">
+        <v>53</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="F156">
         <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:7">
       <c r="A157" t="s">
-        <v>164</v>
+        <v>25</v>
       </c>
       <c r="B157" s="2">
-        <f>VLOOKUP(A157,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C157" t="s">
-        <v>224</v>
+        <v>3</v>
       </c>
       <c r="D157">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F157">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:7">
-      <c r="A158" t="s">
-        <v>25</v>
-      </c>
-      <c r="B158" s="2">
+      <c r="A158" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B158">
+        <v>89</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="F158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" t="s">
+        <v>166</v>
+      </c>
+      <c r="B159" s="2">
+        <f>VLOOKUP(A159,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>126</v>
+      </c>
+      <c r="C159" t="s">
+        <v>76</v>
+      </c>
+      <c r="D159">
         <v>17</v>
       </c>
-      <c r="C158" t="s">
-        <v>3</v>
-      </c>
-      <c r="D158">
-        <v>2</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F158">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7">
-      <c r="A159" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B159">
-        <v>89</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D159">
-        <v>2</v>
+      <c r="E159" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F159">
         <v>1</v>
@@ -4557,37 +4572,39 @@
         <v>126</v>
       </c>
       <c r="C160" t="s">
+        <v>256</v>
+      </c>
+      <c r="D160">
         <v>76</v>
       </c>
-      <c r="D160">
-        <v>17</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F160">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="G160" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
       <c r="B161" s="2">
-        <f>VLOOKUP(A161,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>126</v>
+        <v>24</v>
       </c>
       <c r="C161" t="s">
-        <v>256</v>
+        <v>35</v>
       </c>
       <c r="D161">
-        <v>76</v>
+        <v>35</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F161">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>34</v>
       </c>
@@ -4595,19 +4612,19 @@
         <v>24</v>
       </c>
       <c r="C162" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D162">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>34</v>
       </c>
@@ -4615,19 +4632,19 @@
         <v>24</v>
       </c>
       <c r="C163" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D163">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F163">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
       <c r="A164" t="s">
         <v>34</v>
       </c>
@@ -4635,10 +4652,10 @@
         <v>24</v>
       </c>
       <c r="C164" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="D164">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>87</v>
@@ -4647,7 +4664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>34</v>
       </c>
@@ -4655,10 +4672,10 @@
         <v>24</v>
       </c>
       <c r="C165" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D165">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>87</v>
@@ -4667,7 +4684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>34</v>
       </c>
@@ -4675,10 +4692,10 @@
         <v>24</v>
       </c>
       <c r="C166" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="D166">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>87</v>
@@ -4687,38 +4704,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B167" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C167" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D167">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F167">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="B168" s="2">
-        <v>25</v>
+        <f>VLOOKUP(A168,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>127</v>
       </c>
       <c r="C168" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D168">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>85</v>
@@ -4727,19 +4745,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>9</v>
       </c>
       <c r="B169" s="2">
-        <f>VLOOKUP(A169,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>127</v>
+        <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D169">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>85</v>
@@ -4748,7 +4765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -4756,59 +4773,56 @@
         <v>5</v>
       </c>
       <c r="C170" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D170">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7">
-      <c r="A171" t="s">
-        <v>9</v>
-      </c>
-      <c r="B171" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B171">
+        <v>82</v>
+      </c>
+      <c r="C171" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C171" t="s">
-        <v>3</v>
-      </c>
       <c r="D171">
-        <v>2</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="F171">
-        <v>3</v>
-      </c>
-      <c r="G171" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7">
-      <c r="A172" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B172">
-        <v>82</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" t="s">
+        <v>39</v>
+      </c>
+      <c r="B172" s="2">
+        <v>26</v>
+      </c>
+      <c r="C172" t="s">
+        <v>40</v>
       </c>
       <c r="D172">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F172">
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:6">
       <c r="A173" t="s">
         <v>39</v>
       </c>
@@ -4816,54 +4830,52 @@
         <v>26</v>
       </c>
       <c r="C173" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="D173">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="B174" s="2">
-        <v>26</v>
+        <f>VLOOKUP(A174,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>128</v>
       </c>
       <c r="C174" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="D174">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F174">
-        <v>3</v>
-      </c>
-      <c r="G174" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B175" s="2">
         <f>VLOOKUP(A175,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C175" t="s">
-        <v>78</v>
+        <v>225</v>
       </c>
       <c r="D175">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>85</v>
@@ -4872,7 +4884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:6">
       <c r="A176" t="s">
         <v>169</v>
       </c>
@@ -4881,48 +4893,47 @@
         <v>129</v>
       </c>
       <c r="C176" t="s">
-        <v>225</v>
+        <v>3</v>
       </c>
       <c r="D176">
-        <v>55</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="F176">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177" spans="1:7">
-      <c r="A177" t="s">
-        <v>169</v>
-      </c>
-      <c r="B177" s="2">
-        <f>VLOOKUP(A177,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>129</v>
-      </c>
-      <c r="C177" t="s">
-        <v>3</v>
+      <c r="A177" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B177">
+        <v>83</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D177">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F177">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:7">
-      <c r="A178" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B178">
-        <v>83</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>33</v>
+      <c r="A178" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178" s="2">
+        <v>2</v>
+      </c>
+      <c r="C178" t="s">
+        <v>5</v>
       </c>
       <c r="D178">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F178">
         <v>1</v>
@@ -4936,16 +4947,16 @@
         <v>2</v>
       </c>
       <c r="C179" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="D179">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F179">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -4956,19 +4967,16 @@
         <v>2</v>
       </c>
       <c r="C180" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D180">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>87</v>
       </c>
       <c r="F180">
         <v>3</v>
-      </c>
-      <c r="G180" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -4979,10 +4987,10 @@
         <v>2</v>
       </c>
       <c r="C181" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D181">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>87</v>
@@ -4993,22 +5001,23 @@
     </row>
     <row r="182" spans="1:7">
       <c r="A182" t="s">
-        <v>4</v>
+        <v>170</v>
       </c>
       <c r="B182" s="2">
-        <v>2</v>
+        <f>VLOOKUP(A182,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>131</v>
       </c>
       <c r="C182" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
       <c r="D182">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F182">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -5020,16 +5029,13 @@
         <v>131</v>
       </c>
       <c r="C183" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="D183">
-        <v>38</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="F183">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -5041,10 +5047,10 @@
         <v>131</v>
       </c>
       <c r="C184" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D184">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F184">
         <v>3</v>
@@ -5059,31 +5065,37 @@
         <v>131</v>
       </c>
       <c r="C185" t="s">
-        <v>74</v>
+        <v>227</v>
       </c>
       <c r="D185">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F185">
         <v>3</v>
+      </c>
+      <c r="G185" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="186" spans="1:7">
       <c r="A186" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B186" s="2">
         <f>VLOOKUP(A186,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C186" t="s">
-        <v>227</v>
+        <v>10</v>
       </c>
       <c r="D186">
-        <v>54</v>
+        <v>8</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F186">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -5095,19 +5107,16 @@
         <v>132</v>
       </c>
       <c r="C187" t="s">
-        <v>10</v>
+        <v>226</v>
       </c>
       <c r="D187">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F187">
         <v>1</v>
-      </c>
-      <c r="G187" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -5119,16 +5128,16 @@
         <v>132</v>
       </c>
       <c r="C188" t="s">
-        <v>226</v>
+        <v>38</v>
       </c>
       <c r="D188">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F188">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -5140,49 +5149,52 @@
         <v>132</v>
       </c>
       <c r="C189" t="s">
-        <v>38</v>
+        <v>242</v>
       </c>
       <c r="D189">
-        <v>21</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="F189">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G189" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="190" spans="1:7">
       <c r="A190" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B190" s="2">
         <f>VLOOKUP(A190,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C190" t="s">
-        <v>242</v>
+        <v>123</v>
       </c>
       <c r="D190">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F190">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:7">
       <c r="A191" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B191" s="2">
         <f>VLOOKUP(A191,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C191" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D191">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>85</v>
@@ -5200,43 +5212,37 @@
         <v>134</v>
       </c>
       <c r="C192" t="s">
-        <v>114</v>
+        <v>236</v>
       </c>
       <c r="D192">
-        <v>41</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F192">
-        <v>1</v>
-      </c>
-      <c r="G192" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B193" s="2">
         <f>VLOOKUP(A193,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C193" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="D193">
-        <v>77</v>
+        <v>46</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F193">
-        <v>3</v>
-      </c>
-      <c r="G193" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
       <c r="A194" t="s">
         <v>174</v>
       </c>
@@ -5245,19 +5251,16 @@
         <v>135</v>
       </c>
       <c r="C194" t="s">
-        <v>219</v>
+        <v>3</v>
       </c>
       <c r="D194">
-        <v>46</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="F194">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
       <c r="A195" t="s">
         <v>174</v>
       </c>
@@ -5266,19 +5269,16 @@
         <v>135</v>
       </c>
       <c r="C195" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="D195">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F195">
         <v>3</v>
       </c>
-      <c r="G195" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7">
+    </row>
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
         <v>174</v>
       </c>
@@ -5287,16 +5287,16 @@
         <v>135</v>
       </c>
       <c r="C196" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D196">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F196">
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:6">
       <c r="A197" t="s">
         <v>174</v>
       </c>
@@ -5305,19 +5305,16 @@
         <v>135</v>
       </c>
       <c r="C197" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="D197">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="F197">
         <v>3</v>
       </c>
-      <c r="G197" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7">
+    </row>
+    <row r="198" spans="1:6">
       <c r="A198" t="s">
         <v>174</v>
       </c>
@@ -5326,19 +5323,16 @@
         <v>135</v>
       </c>
       <c r="C198" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="D198">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F198">
         <v>3</v>
       </c>
-      <c r="G198" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7">
+    </row>
+    <row r="199" spans="1:6">
       <c r="A199" t="s">
         <v>174</v>
       </c>
@@ -5347,16 +5341,16 @@
         <v>135</v>
       </c>
       <c r="C199" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D199">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F199">
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:6">
       <c r="A200" t="s">
         <v>174</v>
       </c>
@@ -5365,51 +5359,54 @@
         <v>135</v>
       </c>
       <c r="C200" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D200">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F200">
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
-      <c r="A201" t="s">
-        <v>174</v>
-      </c>
-      <c r="B201" s="2">
-        <f>VLOOKUP(A201,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>135</v>
-      </c>
-      <c r="C201" t="s">
-        <v>260</v>
+    <row r="201" spans="1:6">
+      <c r="A201" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B201">
+        <v>84</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="D201">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="F201">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7">
-      <c r="A202" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B202">
-        <v>84</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>123</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6">
+      <c r="A202" t="s">
+        <v>175</v>
+      </c>
+      <c r="B202" s="2">
+        <f>VLOOKUP(A202,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>136</v>
+      </c>
+      <c r="C202" t="s">
+        <v>3</v>
       </c>
       <c r="D202">
-        <v>42</v>
+        <v>2</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F202">
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:6">
       <c r="A203" t="s">
         <v>175</v>
       </c>
@@ -5418,19 +5415,19 @@
         <v>136</v>
       </c>
       <c r="C203" t="s">
-        <v>3</v>
+        <v>233</v>
       </c>
       <c r="D203">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F203">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
       <c r="A204" t="s">
         <v>175</v>
       </c>
@@ -5438,55 +5435,55 @@
         <f>VLOOKUP(A204,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
         <v>136</v>
       </c>
-      <c r="C204" t="s">
-        <v>233</v>
+      <c r="C204" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="D204">
-        <v>63</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="F204">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
       <c r="A205" t="s">
         <v>175</v>
       </c>
       <c r="B205" s="2">
-        <f>VLOOKUP(A205,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
         <v>136</v>
       </c>
-      <c r="C205" s="5" t="s">
-        <v>195</v>
+      <c r="C205" t="s">
+        <v>233</v>
       </c>
       <c r="D205">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F205">
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:6">
       <c r="A206" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B206" s="2">
-        <v>136</v>
+        <f>VLOOKUP(A206,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>137</v>
       </c>
       <c r="C206" t="s">
-        <v>233</v>
+        <v>3</v>
       </c>
       <c r="D206">
-        <v>63</v>
+        <v>2</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F206">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
       <c r="A207" t="s">
         <v>176</v>
       </c>
@@ -5495,65 +5492,65 @@
         <v>137</v>
       </c>
       <c r="C207" t="s">
-        <v>3</v>
+        <v>237</v>
       </c>
       <c r="D207">
-        <v>2</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F207">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7">
-      <c r="A208" t="s">
-        <v>176</v>
-      </c>
-      <c r="B208" s="2">
-        <f>VLOOKUP(A208,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>137</v>
-      </c>
-      <c r="C208" t="s">
-        <v>237</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
+      <c r="A208" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B208">
+        <v>85</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D208">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="F208">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:7">
       <c r="A209" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B209">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="D209">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="F209">
         <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B210">
-        <v>86</v>
-      </c>
-      <c r="C210" s="3" t="s">
-        <v>114</v>
+      <c r="A210" t="s">
+        <v>177</v>
+      </c>
+      <c r="B210" s="2">
+        <f>VLOOKUP(A210,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>138</v>
+      </c>
+      <c r="C210" t="s">
+        <v>46</v>
       </c>
       <c r="D210">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F210">
         <v>1</v>
@@ -5568,10 +5565,10 @@
         <v>138</v>
       </c>
       <c r="C211" t="s">
-        <v>46</v>
+        <v>228</v>
       </c>
       <c r="D211">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>85</v>
@@ -5589,16 +5586,16 @@
         <v>138</v>
       </c>
       <c r="C212" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D212">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F212">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -5610,16 +5607,13 @@
         <v>138</v>
       </c>
       <c r="C213" t="s">
-        <v>232</v>
+        <v>261</v>
       </c>
       <c r="D213">
-        <v>64</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F213">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -5631,37 +5625,34 @@
         <v>138</v>
       </c>
       <c r="C214" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D214">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F214">
         <v>3</v>
-      </c>
-      <c r="G214" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="215" spans="1:7">
       <c r="A215" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B215" s="2">
         <f>VLOOKUP(A215,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C215" t="s">
-        <v>262</v>
+        <v>76</v>
       </c>
       <c r="D215">
-        <v>84</v>
+        <v>17</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F215">
-        <v>3</v>
-      </c>
-      <c r="G215" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:7">
@@ -5673,48 +5664,50 @@
         <v>139</v>
       </c>
       <c r="C216" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="D216">
-        <v>17</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="F216">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G216" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="217" spans="1:7">
-      <c r="A217" t="s">
-        <v>178</v>
-      </c>
-      <c r="B217" s="2">
-        <f>VLOOKUP(A217,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>139</v>
-      </c>
-      <c r="C217" t="s">
-        <v>3</v>
+      <c r="A217" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B217">
+        <v>54</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="D217">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="F217">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:7">
-      <c r="A218" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B218">
-        <v>54</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>135</v>
+      <c r="A218" t="s">
+        <v>13</v>
+      </c>
+      <c r="B218" s="2">
+        <v>7</v>
+      </c>
+      <c r="C218" t="s">
+        <v>14</v>
       </c>
       <c r="D218">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F218">
         <v>1</v>
@@ -5728,16 +5721,16 @@
         <v>7</v>
       </c>
       <c r="C219" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D219">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F219">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -5748,10 +5741,10 @@
         <v>7</v>
       </c>
       <c r="C220" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D220">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>87</v>
@@ -5768,10 +5761,10 @@
         <v>7</v>
       </c>
       <c r="C221" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="D221">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>87</v>
@@ -5788,10 +5781,10 @@
         <v>7</v>
       </c>
       <c r="C222" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D222">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>87</v>
@@ -5802,45 +5795,43 @@
     </row>
     <row r="223" spans="1:7">
       <c r="A223" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B223" s="2">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C223" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D223">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F223">
-        <v>3</v>
-      </c>
-      <c r="G223" t="s">
-        <v>257</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:7">
       <c r="A224" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="B224" s="2">
-        <v>22</v>
+        <f>VLOOKUP(A224,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>141</v>
       </c>
       <c r="C224" t="s">
-        <v>76</v>
-      </c>
-      <c r="D224">
-        <v>17</v>
+        <v>216</v>
       </c>
       <c r="E224" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F224">
         <v>1</v>
+      </c>
+      <c r="G224" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -5852,7 +5843,10 @@
         <v>141</v>
       </c>
       <c r="C225" t="s">
-        <v>216</v>
+        <v>231</v>
+      </c>
+      <c r="D225">
+        <v>59</v>
       </c>
       <c r="E225" s="1" t="s">
         <v>85</v>
@@ -5870,37 +5864,34 @@
         <v>141</v>
       </c>
       <c r="C226" t="s">
-        <v>231</v>
+        <v>74</v>
       </c>
       <c r="D226">
-        <v>59</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="F226">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="227" spans="1:7">
       <c r="A227" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B227" s="2">
         <f>VLOOKUP(A227,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C227" t="s">
-        <v>74</v>
+        <v>192</v>
       </c>
       <c r="D227">
-        <v>10</v>
+        <v>60</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F227">
-        <v>3</v>
-      </c>
-      <c r="G227" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -5912,19 +5903,13 @@
         <v>142</v>
       </c>
       <c r="C228" t="s">
-        <v>192</v>
+        <v>74</v>
       </c>
       <c r="D228">
-        <v>60</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="F228">
-        <v>1</v>
-      </c>
-      <c r="G228" t="s">
-        <v>212</v>
+        <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -5936,10 +5921,10 @@
         <v>142</v>
       </c>
       <c r="C229" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="D229">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="F229">
         <v>3</v>
@@ -5954,63 +5939,71 @@
         <v>142</v>
       </c>
       <c r="C230" t="s">
-        <v>135</v>
+        <v>227</v>
       </c>
       <c r="D230">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="F230">
         <v>3</v>
       </c>
+      <c r="G230" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" t="s">
-        <v>181</v>
-      </c>
-      <c r="B231" s="2">
-        <f>VLOOKUP(A231,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>142</v>
-      </c>
-      <c r="C231" t="s">
-        <v>227</v>
+      <c r="A231" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B231">
+        <v>87</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D231">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F231">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B232">
-        <v>87</v>
-      </c>
-      <c r="C232" s="3" t="s">
-        <v>75</v>
+      <c r="A232" t="s">
+        <v>182</v>
+      </c>
+      <c r="B232" s="2">
+        <f>VLOOKUP(A232,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>143</v>
+      </c>
+      <c r="C232" t="s">
+        <v>76</v>
       </c>
       <c r="D232">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F232">
         <v>1</v>
+      </c>
+      <c r="G232" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="233" spans="1:7">
       <c r="A233" t="s">
-        <v>182</v>
+        <v>64</v>
       </c>
       <c r="B233" s="2">
-        <f>VLOOKUP(A233,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>143</v>
+        <v>45</v>
       </c>
       <c r="C233" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="D233">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E233" s="1" t="s">
         <v>85</v>
@@ -6027,36 +6020,37 @@
         <v>45</v>
       </c>
       <c r="C234" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D234">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F234">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="235" spans="1:7">
       <c r="A235" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="B235" s="2">
-        <v>45</v>
+        <f>VLOOKUP(A235,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>144</v>
       </c>
       <c r="C235" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
       <c r="D235">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F235">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -6068,34 +6062,36 @@
         <v>144</v>
       </c>
       <c r="C236" t="s">
-        <v>193</v>
+        <v>247</v>
       </c>
       <c r="D236">
-        <v>61</v>
-      </c>
-      <c r="E236" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F236">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G236" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="237" spans="1:7" ht="42">
       <c r="A237" t="s">
-        <v>183</v>
+        <v>11</v>
       </c>
       <c r="B237" s="2">
-        <f>VLOOKUP(A237,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>144</v>
+        <v>6</v>
       </c>
       <c r="C237" t="s">
-        <v>247</v>
+        <v>12</v>
       </c>
       <c r="D237">
+        <v>9</v>
+      </c>
+      <c r="E237" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F237">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -6106,16 +6102,16 @@
         <v>6</v>
       </c>
       <c r="C238" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D238">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F238">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -6126,16 +6122,16 @@
         <v>6</v>
       </c>
       <c r="C239" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D239">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F239">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="240" spans="1:7">
@@ -6146,10 +6142,10 @@
         <v>6</v>
       </c>
       <c r="C240" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="D240">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E240" s="1" t="s">
         <v>87</v>
@@ -6166,10 +6162,10 @@
         <v>6</v>
       </c>
       <c r="C241" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D241">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E241" s="1" t="s">
         <v>87</v>
@@ -6180,40 +6176,38 @@
     </row>
     <row r="242" spans="1:7">
       <c r="A242" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="B242" s="2">
-        <v>6</v>
+        <f>VLOOKUP(A242,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>146</v>
       </c>
       <c r="C242" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="D242">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F242">
-        <v>3</v>
-      </c>
-      <c r="G242" t="s">
-        <v>246</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B243" s="2">
         <f>VLOOKUP(A243,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C243" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="D243">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E243" s="1" t="s">
         <v>85</v>
@@ -6231,10 +6225,10 @@
         <v>145</v>
       </c>
       <c r="C244" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="D244">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E244" s="1" t="s">
         <v>85</v>
@@ -6252,10 +6246,10 @@
         <v>145</v>
       </c>
       <c r="C245" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D245">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E245" s="1" t="s">
         <v>85</v>
@@ -6273,19 +6267,16 @@
         <v>145</v>
       </c>
       <c r="C246" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="D246">
-        <v>2</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F246">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G246" t="s">
-        <v>212</v>
+        <v>248</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -6297,58 +6288,58 @@
         <v>145</v>
       </c>
       <c r="C247" t="s">
-        <v>220</v>
+        <v>74</v>
       </c>
       <c r="D247">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F247">
         <v>3</v>
-      </c>
-      <c r="G247" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="248" spans="1:7">
       <c r="A248" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B248" s="2">
         <f>VLOOKUP(A248,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C248" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="D248">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F248">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G248" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
     </row>
     <row r="249" spans="1:7">
       <c r="A249" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="B249" s="2">
         <f>VLOOKUP(A249,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C249" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="D249">
-        <v>2</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F249">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G249" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -6360,54 +6351,51 @@
         <v>148</v>
       </c>
       <c r="C250" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="D250">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F250">
         <v>3</v>
-      </c>
-      <c r="G250" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="251" spans="1:7">
       <c r="A251" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="B251" s="2">
-        <f>VLOOKUP(A251,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
         <v>148</v>
       </c>
       <c r="C251" t="s">
-        <v>232</v>
+        <v>78</v>
       </c>
       <c r="D251">
-        <v>64</v>
+        <v>20</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F251">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:7">
       <c r="A252" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="B252" s="2">
-        <v>148</v>
+        <f>VLOOKUP(A252,'poets lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>114</v>
       </c>
       <c r="C252" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="D252">
-        <v>20</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="F252">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -6496,8 +6484,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F254">
-    <sortCondition ref="A2"/>
+  <sortState ref="A2:G253">
+    <sortCondition ref="A52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6656,10 +6644,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection sqref="A1:B85"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7359,22 +7347,6 @@
       </c>
       <c r="B83" s="6">
         <v>85</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>265</v>
-      </c>
-      <c r="B84" s="6">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
-        <v>266</v>
-      </c>
-      <c r="B85" s="6">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got rid of highlighting
</commit_message>
<xml_diff>
--- a/production/data/poets_cities.xlsx
+++ b/production/data/poets_cities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="poets" sheetId="1" state="visible" r:id="rId2"/>
@@ -865,18 +865,12 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -930,15 +924,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -978,8 +972,8 @@
   </sheetPr>
   <dimension ref="A1:I258"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="5:6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1088,7 +1082,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" s="3" customFormat="true" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="3" customFormat="true" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1114,7 +1108,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" s="3" customFormat="true" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="3" customFormat="true" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1139,7 +1133,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>20</v>
       </c>
@@ -6221,7 +6215,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="5:6 A2"/>
     </sheetView>
   </sheetViews>
@@ -6373,7 +6367,7 @@
   </sheetPr>
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:6 A1"/>
     </sheetView>
   </sheetViews>
@@ -7137,7 +7131,7 @@
   </sheetPr>
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:6 A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
noted that Messoa was one of four villages that becomes Sparta
</commit_message>
<xml_diff>
--- a/production/data/poets_cities.xlsx
+++ b/production/data/poets_cities.xlsx
@@ -86,7 +86,30 @@
     <t>Messoa</t>
   </si>
   <si>
-    <t> (no location in Pleades)</t>
+    <r>
+      <t>One of villages that becomes Sparta in the 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> c.</t>
+    </r>
   </si>
   <si>
     <t>Sardis</t>
@@ -841,7 +864,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -863,6 +886,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -973,7 +1004,7 @@
   <dimension ref="A1:I258"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:6"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1133,7 +1164,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>20</v>
       </c>
@@ -6216,7 +6247,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="5:6 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -6368,7 +6399,7 @@
   <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -7132,7 +7163,7 @@
   <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>

</xml_diff>